<commit_message>
Fix wrong localization string name
</commit_message>
<xml_diff>
--- a/Workbooks/EN/Environments.xlsx
+++ b/Workbooks/EN/Environments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Workbooks\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A99B2E-2A4C-4042-B38F-4AAE8A30B0B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35E33E2-1736-4B1E-93D0-4F9D1701EF38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Get" sheetId="4" r:id="rId1"/>
     <sheet name="Create" sheetId="1" r:id="rId2"/>
     <sheet name="Delete" sheetId="2" r:id="rId3"/>
-    <sheet name="Add Or Remove Robots" sheetId="6" r:id="rId4"/>
+    <sheet name="Add or Remove Robots" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -736,48 +736,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -926,10 +884,21 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
           <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -956,6 +925,37 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </horizontal>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -970,14 +970,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:E201" headerRowDxfId="15" dataDxfId="23" totalsRowDxfId="14" headerRowBorderDxfId="21" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:E201" headerRowDxfId="23" dataDxfId="21" totalsRowDxfId="19" headerRowBorderDxfId="22" tableBorderDxfId="20">
   <autoFilter ref="A1:E201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Organization Unit ID" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{058B7C0E-F18D-4AA8-A7A4-2A2B65B79498}" name="Organization Unit Name" dataDxfId="19"/>
-    <tableColumn id="1" xr3:uid="{6FFDE20C-2159-4C8B-AE94-46A18EBF32E7}" name="Environment ID" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{81F71C1A-632D-4A5F-BC94-CC97DF7A65EF}" name="Environment Name" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Robots" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Organization Unit ID" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{058B7C0E-F18D-4AA8-A7A4-2A2B65B79498}" name="Organization Unit Name" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{6FFDE20C-2159-4C8B-AE94-46A18EBF32E7}" name="Environment ID" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{81F71C1A-632D-4A5F-BC94-CC97DF7A65EF}" name="Environment Name" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Robots" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>

</xml_diff>

<commit_message>
Implement manipulation of Triggers
</commit_message>
<xml_diff>
--- a/Workbooks/EN/Environments.xlsx
+++ b/Workbooks/EN/Environments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Workbooks\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E80EF3-D867-40BD-8173-5E908A225AAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02AFAB56-E073-4DC0-A686-68570C1FB995}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Get" sheetId="4" r:id="rId1"/>
@@ -2715,7 +2715,7 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Classi Folder ID" error="Classic Folder ID must be an integer greater than 0." sqref="A2:A1048576" xr:uid="{4697A7F3-EE98-42A5-B360-4F5DD4EC3444}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Classic Folder ID" error="Classic Folder ID must be an integer greater than 0." sqref="A2:A1048576" xr:uid="{4697A7F3-EE98-42A5-B360-4F5DD4EC3444}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Environment ID" error="Environment ID must be an integer greater than 0." sqref="C2:C1048576" xr:uid="{E482C9A5-DAF0-4A53-ADC7-9AA1DC33EB48}">
@@ -5407,7 +5407,7 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Classi Folder ID" error="Classic Folder ID must be an integer greater than 0." sqref="A2:A1048576" xr:uid="{FD422441-B078-4B2C-A0B9-34649C5CD378}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Classic Folder ID" error="Classic Folder ID must be an integer greater than 0." sqref="A2:A1048576" xr:uid="{FD422441-B078-4B2C-A0B9-34649C5CD378}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Environment ID" error="Environment ID must be an integer greater than 0." sqref="C2:C1048576" xr:uid="{29F6E9DF-D3FC-4B08-B6C9-D8C81589D199}">

</xml_diff>